<commit_message>
add improvements base on the readme description
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,37 +7,67 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId1" sheetId="1" name="start"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>kind</t>
+  </si>
   <si>
     <t>character</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>animation</t>
+  </si>
+  <si>
     <t>dialogue</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>How are you?</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>option1|otherLabel;option2;option3</t>
+  </si>
+  <si>
     <t>scene</t>
   </si>
   <si>
-    <t>tester1</t>
-  </si>
-  <si>
-    <t>dialog 1</t>
-  </si>
-  <si>
-    <t>first scene</t>
-  </si>
-  <si>
-    <t>tester2</t>
-  </si>
-  <si>
-    <t>dialog 2</t>
+    <t>imageScene</t>
   </si>
 </sst>
 </file>
@@ -45,25 +75,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,14 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -93,16 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -129,28 +137,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -406,15 +414,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -427,28 +440,89 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:construction: add show and hide command
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="start" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t xml:space="preserve">kind</t>
   </si>
@@ -47,6 +47,9 @@
     <t xml:space="preserve">animation</t>
   </si>
   <si>
+    <t xml:space="preserve">hide</t>
+  </si>
+  <si>
     <t xml:space="preserve">dialogue</t>
   </si>
   <si>
@@ -78,6 +81,15 @@
   </si>
   <si>
     <t xml:space="preserve">imageScene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello after scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am angry now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angry</t>
   </si>
   <si>
     <t xml:space="preserve">Hello from another label</t>
@@ -163,20 +175,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -368,10 +384,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,11 +395,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="2" width="13.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="13.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="13.58"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -408,57 +423,114 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -475,18 +547,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="13.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.58"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -511,26 +584,40 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>